<commit_message>
Create MeasureView, Create Quantity/Pages/Measures
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70955864-910B-4C5C-ABDD-C2AF65AC4F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AC0F8E-4540-41C6-89D3-80E77D8040F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>p. 1 tehtud</t>
+  </si>
+  <si>
+    <t>vaatasin 2. video, p. 2 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2332,7 +2335,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2579,15 +2582,29 @@
       <c r="A12" s="31">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="7">
+        <v>43883</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.62291666666666667</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.75347222222222221</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="F12" s="5">
+        <v>188</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="9"/>
+      <c r="J12" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
@@ -2669,7 +2686,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>370</v>
+        <v>558</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Add to Data folder: Common, Docs, Money, Quantity
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AC0F8E-4540-41C6-89D3-80E77D8040F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EAEF7E-715A-4489-BCD6-CD13D911FD99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>vaatasin 2. video, p. 2 tehtud</t>
+  </si>
+  <si>
+    <t>Pluralsight - videokursus</t>
+  </si>
+  <si>
+    <t>Razor Pages in ASP.NET Core: Getting Started (part 1-3)</t>
   </si>
 </sst>
 </file>
@@ -2335,7 +2341,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2345,7 +2351,7 @@
     <col min="3" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
@@ -2610,26 +2616,48 @@
       <c r="A13" s="30">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="B13" s="7">
+        <v>43884</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="E13" s="5">
+        <v>40</v>
+      </c>
+      <c r="F13" s="5">
+        <v>140</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="9"/>
+      <c r="J13" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7">
+        <v>43884</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.6069444444444444</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="9"/>
@@ -2686,7 +2714,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>558</v>
+        <v>698</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Add MeasuresRepository and QuantityDbContext to Infra/Quantity
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EAEF7E-715A-4489-BCD6-CD13D911FD99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB219F6-A16D-4EC6-8CA6-0CCFEE0922A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Razor Pages in ASP.NET Core: Getting Started (part 1-3)</t>
+  </si>
+  <si>
+    <t>p. 3</t>
   </si>
 </sst>
 </file>
@@ -2341,7 +2344,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2652,15 +2655,25 @@
       <c r="C14" s="8">
         <v>0.6069444444444444</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="D14" s="8">
+        <v>0.7680555555555556</v>
+      </c>
+      <c r="E14" s="5">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5">
+        <v>202</v>
+      </c>
       <c r="G14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="I14" s="6"/>
-      <c r="J14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="30">
@@ -2714,7 +2727,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>698</v>
+        <v>900</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Updates in Infra folder, Update in Startup
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB219F6-A16D-4EC6-8CA6-0CCFEE0922A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DD4DF8-47CB-4921-B044-68EFB8347442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="52">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2344,7 +2344,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2679,12 +2679,18 @@
       <c r="A15" s="30">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.50555555555555554</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>

</xml_diff>

<commit_message>
Update MeasuresPage, Create, Delete, details, Edit, Index pages
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DD4DF8-47CB-4921-B044-68EFB8347442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E509FAB1-8814-4455-B85C-B5E1E2C73CC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="52">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2344,7 +2344,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2685,26 +2685,42 @@
       <c r="C15" s="8">
         <v>0.50555555555555554</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="D15" s="8">
+        <v>0.71388888888888891</v>
+      </c>
+      <c r="E15" s="5">
+        <v>60</v>
+      </c>
+      <c r="F15" s="5">
+        <v>240</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="I15" s="6"/>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="31">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="B16" s="7">
+        <v>43885</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="9"/>
@@ -2733,7 +2749,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>900</v>
+        <v>1140</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Fix error in DisplayControlsForHtmlExtension
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B1B4C8-895B-4D40-B2D7-4082E765986E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D91E861-646C-4971-A260-3A04CF2D6D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="54">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2790,7 +2790,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2906,9 +2906,15 @@
       <c r="C7" s="27">
         <v>0.46527777777777773</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="D7" s="27">
+        <v>0.66319444444444442</v>
+      </c>
+      <c r="E7" s="28">
+        <v>90</v>
+      </c>
+      <c r="F7" s="28">
+        <v>195</v>
+      </c>
       <c r="G7" s="34" t="s">
         <v>44</v>
       </c>
@@ -2916,7 +2922,9 @@
         <v>53</v>
       </c>
       <c r="I7" s="25"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
@@ -3068,7 +3076,7 @@
       <c r="E18" s="43"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Create tables in DB
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CB29E6-FFE3-4A10-8F7C-970659D0DB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45346075-B8D0-4D4D-A247-6CE3518501BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="59">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>p. 7 tehtud</t>
+  </si>
+  <si>
+    <t>p. 8 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2805,7 +2808,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3028,15 +3031,29 @@
       <c r="A11" s="30">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="B11" s="7">
+        <v>43890</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.72986111111111107</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.77708333333333324</v>
+      </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="F11" s="5">
+        <v>68</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="I11" s="6"/>
-      <c r="J11" s="9"/>
+      <c r="J11" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="31">
@@ -3132,7 +3149,7 @@
       <c r="E18" s="44"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
-        <v>368</v>
+        <v>436</v>
       </c>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>

</xml_diff>

<commit_message>
Koodi jaotamine repositooriumi klassidesse
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C952AAD7-A59A-4E0D-AC1C-11EE2F43D1B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF3703-E47C-4B1C-B91B-77D25A1E4344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="840" windowWidth="18000" windowHeight="9360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="64">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>p. 12 tehtud</t>
+  </si>
+  <si>
+    <t>alustanud p.13</t>
   </si>
 </sst>
 </file>
@@ -2820,7 +2823,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3185,26 +3188,44 @@
       <c r="A16" s="31">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="7">
+        <v>43892</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0.84722222222222221</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="I16" s="6"/>
-      <c r="J16" s="9"/>
+      <c r="J16" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="30">
         <v>11</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="7">
+        <v>43893</v>
+      </c>
+      <c r="C17" s="19">
+        <v>0.65972222222222221</v>
+      </c>
       <c r="D17" s="19"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
       <c r="J17" s="21"/>

</xml_diff>

<commit_message>
Vaadete mallide (template) jätk
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0444257D-82A7-4AE1-8DFC-2C24A6E361C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9112D3-1227-47EE-B43C-0EA7589457AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="67">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>p.15 tehtud</t>
+  </si>
+  <si>
+    <t>p. 16 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2922,7 +2925,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3378,15 +3381,23 @@
       <c r="C19" s="8">
         <v>0.80972222222222223</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="8">
+        <v>0.86111111111111116</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5">
+        <v>74</v>
+      </c>
       <c r="G19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="9"/>
+      <c r="J19" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="51"/>
@@ -3409,8 +3420,8 @@
       <c r="D21" s="56"/>
       <c r="E21" s="57"/>
       <c r="F21" s="24">
-        <f>SUM(F7:F18)</f>
-        <v>860</v>
+        <f>SUM(F7:F19)</f>
+        <v>934</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
Vaadete mallide (template) lõpp
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9112D3-1227-47EE-B43C-0EA7589457AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E2647-953A-4E12-9A24-8DA37480F643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="68">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>p. 16 tehtud</t>
+  </si>
+  <si>
+    <t>p. 17 tehtud</t>
   </si>
 </sst>
 </file>
@@ -864,7 +867,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -922,6 +924,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1258,68 +1261,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="64">
         <v>43864</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1618,13 +1621,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>852</v>
@@ -1673,68 +1676,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="64">
         <v>43871</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2055,13 +2058,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>884</v>
@@ -2109,68 +2112,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="64">
         <v>43878</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2451,13 +2454,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>834</v>
@@ -2504,68 +2507,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="64">
         <v>43885</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2890,13 +2893,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="57"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>1195</v>
@@ -2922,10 +2925,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9734F-EAA3-493A-90D6-E1A1B4E55705}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2944,68 +2947,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="60"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="61"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="62"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="64" t="s">
+      <c r="B4" s="70"/>
+      <c r="C4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="65">
-        <v>43890</v>
-      </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="66"/>
+      <c r="G4" s="64">
+        <v>43894</v>
+      </c>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="65"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="67"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="69"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3373,7 +3376,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="7">
         <v>43894</v>
@@ -3399,38 +3402,92 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="51">
+        <v>14</v>
+      </c>
+      <c r="B20" s="7">
+        <v>43894</v>
+      </c>
+      <c r="C20" s="40">
+        <v>0.86319444444444438</v>
+      </c>
+      <c r="D20" s="40">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="E20" s="42">
+        <v>20</v>
+      </c>
+      <c r="F20" s="41">
+        <v>122</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="J20" s="43"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="55" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="42"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="43"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="24">
-        <f>SUM(F7:F19)</f>
-        <v>934</v>
-      </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="23"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="24">
+        <f>SUM(F7:F20)</f>
+        <v>1056</v>
+      </c>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>

<commit_message>
SortedRepository (osa 18, 19)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E2647-953A-4E12-9A24-8DA37480F643}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02354559-58D3-4086-A939-0E7E02C6B39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Nädal 3" sheetId="3" r:id="rId3"/>
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
     <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="73">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -273,6 +274,21 @@
   </si>
   <si>
     <t>p. 17 tehtud</t>
+  </si>
+  <si>
+    <t>Kodutöö 6</t>
+  </si>
+  <si>
+    <t>25.03.2020 - 02.03.2020</t>
+  </si>
+  <si>
+    <t>18.02.2020 - 24.02.2020</t>
+  </si>
+  <si>
+    <t>03.03.2020 - 09.03.2020</t>
+  </si>
+  <si>
+    <t>p. 18, 19 tehtud</t>
   </si>
 </sst>
 </file>
@@ -867,6 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -924,7 +941,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1261,68 +1277,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="65">
         <v>43864</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1621,13 +1637,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>852</v>
@@ -1676,68 +1692,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="65">
         <v>43871</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2058,13 +2074,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>884</v>
@@ -2112,68 +2128,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="65">
         <v>43878</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2454,13 +2470,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>834</v>
@@ -2507,68 +2523,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
-        <v>43885</v>
-      </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="G4" s="65" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2893,13 +2909,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>1195</v>
@@ -2927,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9734F-EAA3-493A-90D6-E1A1B4E55705}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2947,68 +2963,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="60"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="64">
-        <v>43894</v>
-      </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="65"/>
+      <c r="G4" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3294,142 +3310,70 @@
       <c r="A16" s="50">
         <v>10</v>
       </c>
-      <c r="B16" s="7">
-        <v>43893</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0.82638888888888884</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0.84722222222222221</v>
-      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5">
-        <v>30</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="50">
         <v>11</v>
       </c>
-      <c r="B17" s="7">
-        <v>43894</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0.71111111111111114</v>
-      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="5">
-        <v>74</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="50">
         <v>12</v>
       </c>
-      <c r="B18" s="7">
-        <v>43894</v>
-      </c>
-      <c r="C18" s="8">
-        <v>0.71597222222222223</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.75138888888888899</v>
-      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5">
-        <v>51</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="50">
         <v>13</v>
       </c>
-      <c r="B19" s="7">
-        <v>43894</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0.80972222222222223</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0.86111111111111116</v>
-      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5">
-        <v>74</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>66</v>
-      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="51">
         <v>14</v>
       </c>
-      <c r="B20" s="7">
-        <v>43894</v>
-      </c>
-      <c r="C20" s="40">
-        <v>0.86319444444444438</v>
-      </c>
-      <c r="D20" s="40">
-        <v>0.96180555555555547</v>
-      </c>
-      <c r="E20" s="42">
-        <v>20</v>
-      </c>
-      <c r="F20" s="41">
-        <v>122</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20" s="42" t="s">
-        <v>16</v>
-      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -3458,7 +3402,7 @@
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="42"/>
-      <c r="B23" s="71"/>
+      <c r="B23" s="52"/>
       <c r="C23" s="40"/>
       <c r="D23" s="40"/>
       <c r="E23" s="42"/>
@@ -3469,16 +3413,476 @@
       <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="57"/>
       <c r="F24" s="24">
         <f>SUM(F7:F20)</f>
-        <v>1056</v>
+        <v>705</v>
+      </c>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A284E252-5A0E-4726-ADCF-9FCEA8ED148D}">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="44">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43893</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <v>30</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43894</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.71111111111111114</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>74</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43894</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5">
+        <v>51</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
+        <v>43894</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
+        <v>74</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7">
+        <v>43894</v>
+      </c>
+      <c r="C11" s="40">
+        <v>0.86319444444444438</v>
+      </c>
+      <c r="D11" s="40">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="E11" s="42">
+        <v>20</v>
+      </c>
+      <c r="F11" s="41">
+        <v>122</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7">
+        <v>43897</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.9375</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5">
+        <v>80</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="50">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="50">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="51">
+        <v>14</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="42"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="43"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="56"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="24">
+        <f>SUM(F7:F20)</f>
+        <v>431</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>

</xml_diff>

<commit_message>
SortedRepository esimesed testid (osa 20)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02354559-58D3-4086-A939-0E7E02C6B39A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C7C4D0-07FB-4D7B-883E-2610CBEA7E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="74">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>p. 18, 19 tehtud</t>
+  </si>
+  <si>
+    <t>p. 20 tehtud</t>
   </si>
 </sst>
 </file>
@@ -3448,7 +3451,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3728,15 +3731,29 @@
       <c r="A13" s="30">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="7">
+        <v>43898</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5.1388888888888894E-2</v>
+      </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="F13" s="5">
+        <v>53</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="9"/>
+      <c r="J13" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
@@ -3882,7 +3899,7 @@
       <c r="E24" s="57"/>
       <c r="F24" s="24">
         <f>SUM(F7:F20)</f>
-        <v>431</v>
+        <v>484</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>

</xml_diff>

<commit_message>
SortedRepository teised testid (osa 21)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C7C4D0-07FB-4D7B-883E-2610CBEA7E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E3411C-7564-4985-904B-8775CB9500D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="75">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>p. 20 tehtud</t>
+  </si>
+  <si>
+    <t>p. 21 tehtud</t>
   </si>
 </sst>
 </file>
@@ -3451,7 +3454,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3759,15 +3762,29 @@
       <c r="A14" s="31">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="7">
+        <v>43898</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.68611111111111101</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="F14" s="5">
+        <v>46</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="I14" s="6"/>
-      <c r="J14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="30">
@@ -3899,7 +3916,7 @@
       <c r="E24" s="57"/>
       <c r="F24" s="24">
         <f>SUM(F7:F20)</f>
-        <v>484</v>
+        <v>530</v>
       </c>
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>

</xml_diff>

<commit_message>
22. osa - SortedRepository testid jätkuvad
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E3411C-7564-4985-904B-8775CB9500D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AA2E69-226E-4468-92CC-99BA7BF0F2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="75">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -3454,7 +3454,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3790,12 +3790,18 @@
       <c r="A15" s="30">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+      <c r="B15" s="7">
+        <v>43899</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>

</xml_diff>

<commit_message>
23. osa - SortedRepository testide lõpp
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AA2E69-226E-4468-92CC-99BA7BF0F2E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58CFA1A-04BA-4B18-91D4-3DFFF0AD4DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Nädal 4" sheetId="4" r:id="rId4"/>
     <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
     <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="78">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -295,6 +296,15 @@
   </si>
   <si>
     <t>p. 21 tehtud</t>
+  </si>
+  <si>
+    <t>10.03.2020 - 16.03.2020</t>
+  </si>
+  <si>
+    <t>p. 22 tehtud, alustanud p. 23</t>
+  </si>
+  <si>
+    <t>p. 23 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2950,7 +2960,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:J4"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3451,10 +3461,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A284E252-5A0E-4726-ADCF-9FCEA8ED148D}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3796,142 +3806,396 @@
       <c r="C15" s="8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="8">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="5">
+        <v>60</v>
+      </c>
       <c r="G15" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="50">
-        <v>10</v>
-      </c>
+      <c r="A16" s="51"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="9"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="50">
-        <v>11</v>
-      </c>
+      <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="50">
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="50">
-        <v>13</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="51">
-        <v>14</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="43"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="43"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="43"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="42"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="43"/>
-    </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="24">
-        <f>SUM(F7:F20)</f>
-        <v>530</v>
-      </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="23"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="24">
+        <f>SUM(F7:F15)</f>
+        <v>590</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD72131-D814-4251-9F7D-944E6AC615A7}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="60"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="70" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="71"/>
+      <c r="C4" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="66"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="54"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="44">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43893</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.82986111111111116</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.87777777777777777</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <v>69</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="42"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="24">
+        <f>SUM(F7:F15)</f>
+        <v>69</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>

<commit_message>
Repository klasside refaktoorimine  (osa 24)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DFD537-A40E-4BC4-9647-E8F32F9FE863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5386D359-5F9B-49A4-B2EF-AFC58F3427CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="80">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>alustanud p.24</t>
+  </si>
+  <si>
+    <t>p. 24 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2962,7 +2965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B9734F-EAA3-493A-90D6-E1A1B4E55705}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -3897,7 +3900,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4063,15 +4066,29 @@
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="7">
+        <v>43901</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.96319444444444446</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="F9" s="5">
+        <v>42</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
@@ -4203,7 +4220,7 @@
       <c r="E19" s="57"/>
       <c r="F19" s="24">
         <f>SUM(F7:F15)</f>
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>

</xml_diff>

<commit_message>
Repository klasside kokkuvõte  (osa 25)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF603BB6-E618-44EA-8F28-0ED07B7EC20E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654C9B66-CF28-41B0-A44B-7FF3D89C050D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="82">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>alustanud p. 25</t>
+  </si>
+  <si>
+    <t>p.25 tehtud</t>
   </si>
 </sst>
 </file>
@@ -3903,7 +3906,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4125,29 +4128,55 @@
       <c r="A11" s="30">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="B11" s="7">
+        <v>43902</v>
+      </c>
+      <c r="C11" s="40">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D11" s="40">
+        <v>0.375</v>
+      </c>
       <c r="E11" s="42"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="41">
+        <v>60</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="H11" s="6"/>
-      <c r="I11" s="42"/>
+      <c r="I11" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="31">
         <v>6</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="B12" s="7">
+        <v>43902</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.40833333333333338</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="F12" s="5">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="9"/>
+      <c r="J12" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="30">
@@ -4237,7 +4266,7 @@
       <c r="E19" s="57"/>
       <c r="F19" s="24">
         <f>SUM(F7:F15)</f>
-        <v>151</v>
+        <v>229</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>

</xml_diff>

<commit_message>
FilteredRepository universaalseks (osa 26)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654C9B66-CF28-41B0-A44B-7FF3D89C050D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC5DA3-4030-4E5A-B146-E860D20B715A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="83">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>p.25 tehtud</t>
+  </si>
+  <si>
+    <t>p. 26 tehtud</t>
   </si>
 </sst>
 </file>
@@ -3906,7 +3909,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4182,15 +4185,29 @@
       <c r="A13" s="30">
         <v>7</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="B13" s="7">
+        <v>43902</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.40902777777777777</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.43263888888888885</v>
+      </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="F13" s="5">
+        <v>33</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="9"/>
+      <c r="J13" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="31">
@@ -4266,7 +4283,7 @@
       <c r="E19" s="57"/>
       <c r="F19" s="24">
         <f>SUM(F7:F15)</f>
-        <v>229</v>
+        <v>262</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>

</xml_diff>

<commit_message>
Lambda Expression selgitused (osa 27)
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC5DA3-4030-4E5A-B146-E860D20B715A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494327BE-D725-44B7-BDD5-EB6512D1354D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="84">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>p. 26 tehtud</t>
+  </si>
+  <si>
+    <t>p. 27 tehtud</t>
   </si>
 </sst>
 </file>
@@ -4213,14 +4216,28 @@
       <c r="A14" s="31">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="7">
+        <v>43902</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.43402777777777773</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.4513888888888889</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="F14" s="5">
+        <v>25</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -4283,7 +4300,7 @@
       <c r="E19" s="57"/>
       <c r="F19" s="24">
         <f>SUM(F7:F15)</f>
-        <v>262</v>
+        <v>287</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>

</xml_diff>

<commit_message>
MeasuresPageModel Edit, Create, Details ja Delete refaktoorimine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494327BE-D725-44B7-BDD5-EB6512D1354D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FFCCE9-90E2-4357-8508-5573F8AE1DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="88">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -323,6 +323,18 @@
   </si>
   <si>
     <t>p. 27 tehtud</t>
+  </si>
+  <si>
+    <t>Raamatu lugemine</t>
+  </si>
+  <si>
+    <t>Clean Code</t>
+  </si>
+  <si>
+    <t>Kodutöö 7</t>
+  </si>
+  <si>
+    <t>p. 28 tehtud</t>
   </si>
 </sst>
 </file>
@@ -3912,7 +3924,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4244,39 +4256,85 @@
       <c r="A15" s="30">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="7">
+        <v>43904</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="F15" s="5">
+        <v>120</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="I15" s="6"/>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="A16" s="51">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7">
+        <v>43905</v>
+      </c>
+      <c r="C16" s="40">
+        <v>0.9375</v>
+      </c>
+      <c r="D16" s="40">
+        <v>0.98958333333333337</v>
+      </c>
       <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="42"/>
+      <c r="F16" s="41">
+        <v>75</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="I16" s="42"/>
-      <c r="J16" s="43"/>
+      <c r="J16" s="43" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="6">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7">
+        <v>43906</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.71666666666666667</v>
+      </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="42"/>
+      <c r="F17" s="5">
+        <v>62</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>87</v>
+      </c>
       <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="J17" s="43" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="42"/>
@@ -4299,8 +4357,8 @@
       <c r="D19" s="56"/>
       <c r="E19" s="57"/>
       <c r="F19" s="24">
-        <f>SUM(F7:F15)</f>
-        <v>287</v>
+        <f>SUM(F7:F17)</f>
+        <v>544</v>
       </c>
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>

</xml_diff>

<commit_message>
29. osa - MeasuresPageModel Index asjade refaktoorimine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FFCCE9-90E2-4357-8508-5573F8AE1DEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B853AB7-58D2-4233-BFE3-A137D27A75EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="89">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t>p. 28 tehtud</t>
+  </si>
+  <si>
+    <t>p. 29 tehtud</t>
   </si>
 </sst>
 </file>
@@ -382,7 +385,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -848,11 +851,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -987,6 +1001,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -3921,10 +3936,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD72131-D814-4251-9F7D-944E6AC615A7}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4336,38 +4351,80 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="42"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="42">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7">
+        <v>43906</v>
+      </c>
+      <c r="C18" s="40">
+        <v>0.71805555555555556</v>
+      </c>
+      <c r="D18" s="40">
+        <v>0.7583333333333333</v>
+      </c>
       <c r="E18" s="42"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="F18" s="41">
+        <v>58</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>88</v>
+      </c>
       <c r="I18" s="42"/>
-      <c r="J18" s="43"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="55" t="s">
+      <c r="J18" s="43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="42"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="72" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="24">
-        <f>SUM(F7:F17)</f>
-        <v>544</v>
-      </c>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="23"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="24">
+        <f>SUM(F7:F19)</f>
+        <v>602</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A21:E21"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>

<commit_message>
30. osa - BasePageModel lisamine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FECE8A-B0F8-49F6-ACC4-EF46DB0D84FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DF7B5D-FF24-435D-8DE9-17E3B8896CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Nädal 5" sheetId="5" r:id="rId5"/>
     <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
     <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="92">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -341,6 +342,12 @@
   </si>
   <si>
     <t>p. 30 - jäi vea tõttu pooleli</t>
+  </si>
+  <si>
+    <t>17.03.2020 - 23.03.2020</t>
+  </si>
+  <si>
+    <t>p. 30 tehtud</t>
   </si>
 </sst>
 </file>
@@ -388,7 +395,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -865,11 +872,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -948,6 +970,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1341,68 +1365,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="68">
         <v>43864</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1701,13 +1725,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>852</v>
@@ -1756,68 +1780,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="68">
         <v>43871</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2138,13 +2162,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>884</v>
@@ -2192,68 +2216,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="68">
         <v>43878</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2534,13 +2558,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>834</v>
@@ -2587,68 +2611,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2973,13 +2997,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="58"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>1195</v>
@@ -3027,68 +3051,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3477,13 +3501,13 @@
       <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="56" t="s">
+      <c r="A24" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="58"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="60"/>
       <c r="F24" s="24">
         <f>SUM(F7:F20)</f>
         <v>705</v>
@@ -3531,68 +3555,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3907,13 +3931,13 @@
       <c r="J18" s="43"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="24">
         <f>SUM(F7:F15)</f>
         <v>590</v>
@@ -3941,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD72131-D814-4251-9F7D-944E6AC615A7}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3961,68 +3985,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="64"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="65" t="s">
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -4422,16 +4446,366 @@
       <c r="I20" s="42"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
         <v>741</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99488E6F-0C7F-4F69-B512-A71E5909B9EA}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="64"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="66"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="74"/>
+      <c r="C4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="69"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="72"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="44">
+        <v>1</v>
+      </c>
+      <c r="B7" s="45">
+        <v>43907</v>
+      </c>
+      <c r="C7" s="46">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.71388888888888891</v>
+      </c>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47">
+        <v>24</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="51">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="51">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="53"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="24">
+        <f>SUM(F7:F19)</f>
+        <v>24</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
31. osa - Testimise abifunktsioonide lisamine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DF7B5D-FF24-435D-8DE9-17E3B8896CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874AC12E-C993-467D-A86F-E4CCAD548D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="93">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>p. 30 tehtud</t>
+  </si>
+  <si>
+    <t>p. 31 tehtud</t>
   </si>
 </sst>
 </file>
@@ -357,7 +360,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +388,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4481,7 +4490,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4587,7 +4596,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="44">
         <v>1</v>
       </c>
@@ -4619,15 +4628,29 @@
       <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="45">
+        <v>43907</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.75208333333333333</v>
+      </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="5">
+        <v>53</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
@@ -4805,7 +4828,7 @@
       <c r="E21" s="60"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
@@ -4822,6 +4845,7 @@
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
32. osa - Testid korda
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874AC12E-C993-467D-A86F-E4CCAD548D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234FDFDC-E465-46E7-9A47-8A9768B17A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="94">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>p. 31 tehtud</t>
+  </si>
+  <si>
+    <t>p. 32 tehtud</t>
   </si>
 </sst>
 </file>
@@ -4490,7 +4493,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4624,7 +4627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31">
         <v>2</v>
       </c>
@@ -4656,15 +4659,29 @@
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="B9" s="45">
+        <v>43907</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="F9" s="5">
+        <v>135</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
@@ -4828,7 +4845,7 @@
       <c r="E21" s="60"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>77</v>
+        <v>212</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
33. osa - DropDown valiku loomine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234FDFDC-E465-46E7-9A47-8A9768B17A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8B6E50-7DF8-4736-B51D-8AD1771A19F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4493,7 +4493,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4687,8 +4687,12 @@
       <c r="A10" s="31">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="7">
+        <v>43908</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.77430555555555547</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>

</xml_diff>

<commit_message>
35. osa - Master-detail seos
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8B6E50-7DF8-4736-B51D-8AD1771A19F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05643DD4-61AB-4A63-854F-E8F4E8549318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="95">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>p. 32 tehtud</t>
+  </si>
+  <si>
+    <t>p. 33, 34, 35 tehtud</t>
   </si>
 </sst>
 </file>
@@ -4493,7 +4496,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4655,7 +4658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30">
         <v>3</v>
       </c>
@@ -4693,13 +4696,25 @@
       <c r="C10" s="8">
         <v>0.77430555555555547</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="D10" s="8">
+        <v>0.94791666666666663</v>
+      </c>
+      <c r="E10" s="5">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5">
+        <v>220</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="30">
@@ -4849,7 +4864,7 @@
       <c r="E21" s="60"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>212</v>
+        <v>432</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
36. osa - Master-detail tööle
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05643DD4-61AB-4A63-854F-E8F4E8549318}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C226A43A-19B3-4E6D-8C75-8BF2273D3AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="96">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t>p. 33, 34, 35 tehtud</t>
+  </si>
+  <si>
+    <t>p. 36 tehtud</t>
   </si>
 </sst>
 </file>
@@ -4496,7 +4499,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4686,7 +4689,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31">
         <v>4</v>
       </c>
@@ -4720,14 +4723,28 @@
       <c r="A11" s="30">
         <v>5</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
+      <c r="B11" s="7">
+        <v>43909</v>
+      </c>
+      <c r="C11" s="40">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D11" s="40">
+        <v>0.84027777777777779</v>
+      </c>
       <c r="E11" s="42"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="42"/>
+      <c r="F11" s="41">
+        <v>190</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -4864,7 +4881,7 @@
       <c r="E21" s="60"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>432</v>
+        <v>622</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
osa 37 - Master-detail lõpetamine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C226A43A-19B3-4E6D-8C75-8BF2273D3AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42856D71-8670-4065-BFC3-E8B1312A4128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Nädal 6" sheetId="6" r:id="rId6"/>
     <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
+    <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="98">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -360,6 +361,12 @@
   </si>
   <si>
     <t>p. 36 tehtud</t>
+  </si>
+  <si>
+    <t>24.03.2020 - 30.03.2020</t>
+  </si>
+  <si>
+    <t>p. 37 tehtud</t>
   </si>
 </sst>
 </file>
@@ -413,7 +420,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -905,11 +912,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -990,6 +1010,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1383,68 +1405,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="70">
         <v>43864</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1743,13 +1765,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>852</v>
@@ -1798,68 +1820,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="70">
         <v>43871</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2180,13 +2202,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>884</v>
@@ -2234,68 +2256,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="70">
         <v>43878</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -2576,13 +2598,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>834</v>
@@ -2629,68 +2651,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3015,13 +3037,13 @@
       <c r="J17" s="21"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="24">
         <f>SUM(F7:F17)</f>
         <v>1195</v>
@@ -3069,68 +3091,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3519,13 +3541,13 @@
       <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="62"/>
       <c r="F24" s="24">
         <f>SUM(F7:F20)</f>
         <v>705</v>
@@ -3573,68 +3595,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -3949,13 +3971,13 @@
       <c r="J18" s="43"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="62"/>
       <c r="F19" s="24">
         <f>SUM(F7:F15)</f>
         <v>590</v>
@@ -4003,68 +4025,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -4464,13 +4486,13 @@
       <c r="I20" s="42"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
         <v>741</v>
@@ -4498,8 +4520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99488E6F-0C7F-4F69-B512-A71E5909B9EA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4518,68 +4540,68 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="66"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="67" t="s">
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="72"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="57"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
@@ -4872,13 +4894,13 @@
       <c r="J20" s="55"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="60"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
         <v>622</v>
@@ -4901,4 +4923,354 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49A5DCE-A753-461C-89B5-7B2FB2A5832F}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="44">
+        <v>1</v>
+      </c>
+      <c r="B7" s="57">
+        <v>43915</v>
+      </c>
+      <c r="C7" s="46">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47">
+        <v>82</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="51">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="51">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="53"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="24">
+        <f>SUM(F7:F19)</f>
+        <v>82</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
38. osa - Master-detail refaktoorimine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42856D71-8670-4065-BFC3-E8B1312A4128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D03832A-7FB2-4FAF-A7A5-DB1352E80171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="100">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -367,6 +367,12 @@
   </si>
   <si>
     <t>p. 37 tehtud</t>
+  </si>
+  <si>
+    <t>Kodutöö 8</t>
+  </si>
+  <si>
+    <t>p. 38 tehtud</t>
   </si>
 </sst>
 </file>
@@ -4929,8 +4935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49A5DCE-A753-461C-89B5-7B2FB2A5832F}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5036,7 +5042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="44">
         <v>1</v>
       </c>
@@ -5054,7 +5060,7 @@
         <v>82</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>97</v>
@@ -5068,15 +5074,31 @@
       <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="B8" s="57">
+        <v>43915</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E8" s="5">
+        <v>40</v>
+      </c>
+      <c r="F8" s="5">
+        <v>230</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
@@ -5254,7 +5276,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>82</v>
+        <v>312</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
HtmlExtension meetodite testide raamistikud -started
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D03832A-7FB2-4FAF-A7A5-DB1352E80171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9F3932-40ED-4C7E-99FB-DD4BB0F12AA2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,16 +23,10 @@
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
     <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -73,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="100">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -4936,7 +4930,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5070,7 +5064,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31">
         <v>2</v>
       </c>
@@ -5104,12 +5098,18 @@
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="26">
+        <v>43916</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.6875</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="56" t="s">
+        <v>98</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>

</xml_diff>

<commit_message>
39. osa - HtmlExtension meetodite testide raamistikud - tehtud
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9F3932-40ED-4C7E-99FB-DD4BB0F12AA2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D72F41-A47A-4E41-9FC5-48E4A9584E82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="101">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>p. 38 tehtud</t>
+  </si>
+  <si>
+    <t>p. 39 - alustanud</t>
   </si>
 </sst>
 </file>
@@ -4930,7 +4933,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5064,7 +5067,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>2</v>
       </c>
@@ -5083,7 +5086,7 @@
       <c r="F8" s="5">
         <v>230</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="6" t="s">
         <v>98</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -5104,26 +5107,40 @@
       <c r="C9" s="8">
         <v>0.6875</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="56" t="s">
+      <c r="F9" s="5">
+        <v>30</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>4</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="26">
+        <v>43916</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.8125</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
@@ -5276,7 +5293,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>312</v>
+        <v>342</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
45. osa - Quantity Data Model
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B94D2D6-94C2-4149-A97C-1B3B445D48CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CADC13B-10B8-4378-9A8F-F5B9CF506D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="106">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>vigade parandamine, kodutöö 8 tehtud</t>
+  </si>
+  <si>
+    <t>Kodutöö 9</t>
   </si>
 </sst>
 </file>
@@ -4951,7 +4954,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5259,12 +5262,18 @@
       <c r="A14" s="31">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="7">
+        <v>43919</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="9"/>

</xml_diff>

<commit_message>
48 osa - pooleli
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E5DB2E-A201-4105-BDDE-D752965A7DDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCEBDA1-16A5-47A6-A008-49B17D7A6BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="108">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>p. 45-47 tehtud</t>
+  </si>
+  <si>
+    <t>48 osa - pooleli</t>
   </si>
 </sst>
 </file>
@@ -4957,7 +4960,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5293,15 +5296,29 @@
       <c r="A15" s="30">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="7">
+        <v>43920</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.94444444444444453</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="F15" s="5">
+        <v>120</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="I15" s="6"/>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="51">
@@ -5381,7 +5398,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>943</v>
+        <v>1063</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
48. osa - Quantity Facade testid ja klassid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCEBDA1-16A5-47A6-A008-49B17D7A6BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7A43F0-3FB8-43FB-8E36-7B07F82AFF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Nädal 7" sheetId="7" r:id="rId7"/>
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
     <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
+    <sheet name="Nädal 10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="110">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -397,6 +398,12 @@
   </si>
   <si>
     <t>48 osa - pooleli</t>
+  </si>
+  <si>
+    <t>31.03.2020 - 06.04.2020</t>
+  </si>
+  <si>
+    <t>p. 48 tehtud</t>
   </si>
 </sst>
 </file>
@@ -1826,6 +1833,356 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2CEA36-23FE-43FD-BFAB-853AFC9EC1D8}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="44">
+        <v>1</v>
+      </c>
+      <c r="B7" s="57">
+        <v>43911</v>
+      </c>
+      <c r="C7" s="46">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.56041666666666667</v>
+      </c>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47">
+        <v>72</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="57"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="51">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="51">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="53"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="24">
+        <f>SUM(F7:F19)</f>
+        <v>72</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E639A5B4-1857-4E5D-8A42-CEA038C67138}">
   <dimension ref="A1:J18"/>
@@ -4551,7 +4908,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4959,8 +5316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49A5DCE-A753-461C-89B5-7B2FB2A5832F}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
49. osa - Infra BaseRepository testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3C6488-4836-4DC5-BBB0-A033A3F1D038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C268E2F8-EC4F-405F-B98C-120AA03817CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="111">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1841,7 +1841,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,7 +1947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="44">
         <v>1</v>
       </c>
@@ -1979,7 +1979,7 @@
       <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="7">
         <v>43911</v>
       </c>
       <c r="C8" s="8">
@@ -1992,7 +1992,7 @@
       <c r="F8" s="5">
         <v>22</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="6" t="s">
         <v>105</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -2007,12 +2007,18 @@
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="7">
+        <v>43911</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.74305555555555547</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>

</xml_diff>

<commit_message>
50. osa - Infra FilteredRepository testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C268E2F8-EC4F-405F-B98C-120AA03817CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E646D3F8-59C0-4233-9E77-91A60F7FE681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="112">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>p. 49 - alustanud</t>
+  </si>
+  <si>
+    <t>p. 49-50 tehtud</t>
   </si>
 </sst>
 </file>
@@ -1841,7 +1844,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2013,15 +2016,25 @@
       <c r="C9" s="8">
         <v>0.74305555555555547</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="8">
+        <v>0.95277777777777783</v>
+      </c>
+      <c r="E9" s="5">
+        <v>60</v>
+      </c>
+      <c r="F9" s="5">
+        <v>242</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="9"/>
+      <c r="J9" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
@@ -2185,7 +2198,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>94</v>
+        <v>336</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
51. osa - Infra PaginatedRepository testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E646D3F8-59C0-4233-9E77-91A60F7FE681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7D479F-2E64-45A9-B17E-E797E6A8FB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="112">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1844,7 +1844,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,7 +1955,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="57">
-        <v>43911</v>
+        <v>43921</v>
       </c>
       <c r="C7" s="46">
         <v>0.51041666666666663</v>
@@ -1983,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="7">
-        <v>43911</v>
+        <v>43921</v>
       </c>
       <c r="C8" s="8">
         <v>0.5625</v>
@@ -2011,7 +2011,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="7">
-        <v>43911</v>
+        <v>43921</v>
       </c>
       <c r="C9" s="8">
         <v>0.74305555555555547</v>
@@ -2040,12 +2040,18 @@
       <c r="A10" s="31">
         <v>4</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="8"/>
+      <c r="B10" s="26">
+        <v>43922</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.71875</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>

</xml_diff>

<commit_message>
52. osa - Infra MeasuresRepository testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7D479F-2E64-45A9-B17E-E797E6A8FB93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7518E6B1-4B33-40A4-AFC2-96F31995EEF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="113">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>p. 49-50 tehtud</t>
+  </si>
+  <si>
+    <t>p.51-52 tehtud</t>
   </si>
 </sst>
 </file>
@@ -1844,7 +1847,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2046,13 +2049,21 @@
       <c r="C10" s="8">
         <v>0.71875</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="D10" s="8">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="E10" s="5">
+        <v>60</v>
+      </c>
+      <c r="F10" s="5">
+        <v>195</v>
+      </c>
       <c r="G10" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
     </row>
@@ -2204,7 +2215,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>336</v>
+        <v>531</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
53. osa - Infra QuantityDbContext testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB898D6-B364-45B9-8DAF-743E26D7E3D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BE491B-A0F1-4726-B2AE-10EC2696B764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="120">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -425,6 +425,15 @@
   </si>
   <si>
     <t>Trello</t>
+  </si>
+  <si>
+    <t>Kontrolltöö</t>
+  </si>
+  <si>
+    <t>Kodutöö 10</t>
+  </si>
+  <si>
+    <t>p. 53 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2167,29 +2176,55 @@
       <c r="A14" s="31">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="7">
+        <v>43925</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.55902777777777779</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="6"/>
+      <c r="F14" s="5">
+        <v>30</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="I14" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="30">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="B15" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.56041666666666667</v>
+      </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="F15" s="5">
+        <v>57</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="I15" s="6"/>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="51">
@@ -2269,7 +2304,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>671</v>
+        <v>758</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
54. osa - Infra QuantityDbInitializer testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BE491B-A0F1-4726-B2AE-10EC2696B764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F988B299-5C73-4465-963B-9F323CC04EDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="121">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>p. 53 tehtud</t>
+  </si>
+  <si>
+    <t>p. 54 tehtud</t>
   </si>
 </sst>
 </file>
@@ -1868,7 +1871,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2230,15 +2233,31 @@
       <c r="A16" s="51">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C16" s="40">
+        <v>0.57222222222222219</v>
+      </c>
+      <c r="D16" s="40">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="E16" s="41">
+        <v>40</v>
+      </c>
+      <c r="F16" s="41">
+        <v>106</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="I16" s="42"/>
-      <c r="J16" s="43"/>
+      <c r="J16" s="43" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="50">
@@ -2304,7 +2323,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>758</v>
+        <v>864</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
55. osa - Infra UnitsRepository testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F988B299-5C73-4465-963B-9F323CC04EDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F778043E-526A-4E80-A0CE-7F488C1D21A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="122">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>p. 54 tehtud</t>
+  </si>
+  <si>
+    <t>p. 55 tehtud</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1874,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2263,15 +2266,29 @@
       <c r="A17" s="50">
         <v>11</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.90972222222222221</v>
+      </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="42"/>
+      <c r="F17" s="5">
+        <v>80</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H17" s="42" t="s">
+        <v>121</v>
+      </c>
       <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="J17" s="43" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="51">
@@ -2323,7 +2340,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>864</v>
+        <v>944</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
56. osa - Infra teised Quantity repositooriumid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F778043E-526A-4E80-A0CE-7F488C1D21A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D31B93E-E361-4BA4-9DD6-E46993136A2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="123">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>p. 55 tehtud</t>
+  </si>
+  <si>
+    <t>p. 56 tehtud</t>
   </si>
 </sst>
 </file>
@@ -1874,7 +1877,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2294,29 +2297,55 @@
       <c r="A18" s="51">
         <v>12</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
+      <c r="B18" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C18" s="40">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="D18" s="40">
+        <v>0.92708333333333337</v>
+      </c>
       <c r="E18" s="42"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="6"/>
+      <c r="F18" s="41">
+        <v>20</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="I18" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="J18" s="43"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="50">
         <v>13</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="B19" s="7">
+        <v>43926</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.95138888888888884</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.98611111111111116</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="F19" s="5">
+        <v>50</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="I19" s="6"/>
-      <c r="J19" s="53"/>
+      <c r="J19" s="53" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="54"/>
@@ -2340,7 +2369,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>944</v>
+        <v>1014</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
57. osa - Infra Quantity repositooriumite testid
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D31B93E-E361-4BA4-9DD6-E46993136A2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EE04F-A38D-41C8-9747-1660230B2CE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Nädal 8" sheetId="8" r:id="rId8"/>
     <sheet name="Nädal 9" sheetId="9" r:id="rId9"/>
     <sheet name="Nädal 10" sheetId="10" r:id="rId10"/>
+    <sheet name="Nädal 11" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="124">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -442,7 +443,10 @@
     <t>p. 55 tehtud</t>
   </si>
   <si>
-    <t>p. 56 tehtud</t>
+    <t>p. 56, 57 tehtud</t>
+  </si>
+  <si>
+    <t>07.04.2020 - 13.04.2020</t>
   </si>
 </sst>
 </file>
@@ -1877,7 +1881,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2330,11 +2334,11 @@
         <v>0.95138888888888884</v>
       </c>
       <c r="D19" s="8">
-        <v>0.98611111111111116</v>
+        <v>2.7777777777777779E-3</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>118</v>
@@ -2369,7 +2373,343 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>1014</v>
+        <v>1048</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85020F5-35D7-4E4C-8099-C735F0FD7214}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="73.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="68"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="76"/>
+      <c r="C4" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="71"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="74"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="44">
+        <v>1</v>
+      </c>
+      <c r="B7" s="57"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="30">
+        <v>3</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>4</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="31">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="30">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="51">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="50">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="51">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="50">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="53"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="54"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="24">
+        <f>SUM(F7:F19)</f>
+        <v>0</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
58. osa - Uued lehed ja view'd
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923EE04F-A38D-41C8-9747-1660230B2CE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6328A4-5561-4129-B280-8A9A6AC0F21A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="124">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2CEA36-23FE-43FD-BFAB-853AFC9EC1D8}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2398,8 +2398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85020F5-35D7-4E4C-8099-C735F0FD7214}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2509,12 +2509,22 @@
       <c r="A7" s="44">
         <v>1</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
+      <c r="B7" s="57">
+        <v>43929</v>
+      </c>
+      <c r="C7" s="46">
+        <v>0.9375</v>
+      </c>
+      <c r="D7" s="46">
+        <v>1.1805555555555555E-2</v>
+      </c>
       <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="56"/>
+      <c r="F7" s="47">
+        <v>107</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>118</v>
+      </c>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
@@ -2709,7 +2719,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
started 59. osa - Uute lehtede ja vaadete testimine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6328A4-5561-4129-B280-8A9A6AC0F21A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46450AAE-5CB1-4CB6-989A-326666DFB953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="126">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>07.04.2020 - 13.04.2020</t>
+  </si>
+  <si>
+    <t>p. 58 tehtud</t>
+  </si>
+  <si>
+    <t>p. 59 - alustanud</t>
   </si>
 </sst>
 </file>
@@ -2399,7 +2405,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2505,7 +2511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="44">
         <v>1</v>
       </c>
@@ -2525,23 +2531,41 @@
       <c r="G7" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="16" t="s">
+        <v>124</v>
+      </c>
       <c r="I7" s="16"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="B8" s="57">
+        <v>43930</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2.4305555555555556E-2</v>
+      </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="5">
+        <v>14</v>
+      </c>
+      <c r="G8" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="I8" s="6"/>
-      <c r="J8" s="9"/>
+      <c r="J8" s="9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
@@ -2719,7 +2743,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>

<commit_message>
59. osa - Uute lehtede ja vaadete testimine (lõpetatud) 60. osa - Page baasklasside testimine
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46450AAE-5CB1-4CB6-989A-326666DFB953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43AA119-2E17-4B3D-8E38-0172FE508DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="126">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -2405,7 +2405,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,7 +2539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31">
         <v>2</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="F8" s="5">
         <v>14</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="6" t="s">
         <v>118</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -2571,12 +2571,18 @@
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="B9" s="57">
+        <v>43930</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="9"/>

</xml_diff>

<commit_message>
62. osa - DropDown lisamine Create vaadetele
</commit_message>
<xml_diff>
--- a/Time recording log.xlsx
+++ b/Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Homework4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43AA119-2E17-4B3D-8E38-0172FE508DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7D2551-9E10-4E08-A399-42374AAE949F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="127">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>p. 59 - alustanud</t>
+  </si>
+  <si>
+    <t>p. 59 - 62 tehtud</t>
   </si>
 </sst>
 </file>
@@ -2405,7 +2408,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2511,7 +2514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="44">
         <v>1</v>
       </c>
@@ -2539,11 +2542,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>2</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="26">
         <v>43930</v>
       </c>
       <c r="C8" s="8">
@@ -2571,20 +2574,30 @@
       <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="26">
         <v>43930</v>
       </c>
       <c r="C9" s="8">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="D9" s="8">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="E9" s="5">
+        <v>20</v>
+      </c>
+      <c r="F9" s="5">
+        <v>300</v>
+      </c>
       <c r="G9" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="H9" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2749,7 +2762,7 @@
       <c r="E21" s="62"/>
       <c r="F21" s="24">
         <f>SUM(F7:F19)</f>
-        <v>121</v>
+        <v>421</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>

</xml_diff>